<commit_message>
Updated LMSR for Insurance
</commit_message>
<xml_diff>
--- a/docs/LogMSR_Demo.xlsx
+++ b/docs/LogMSR_Demo.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="21075" windowHeight="9975"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="21075" windowHeight="9975" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HLMSR" sheetId="6" r:id="rId1"/>
     <sheet name="Changing b mid contract" sheetId="8" r:id="rId2"/>
-    <sheet name="Some Accounting" sheetId="7" r:id="rId3"/>
-    <sheet name="2x2 Update Calculator" sheetId="5" r:id="rId4"/>
+    <sheet name="Insurance Fraud" sheetId="9" r:id="rId3"/>
+    <sheet name="Some Accounting" sheetId="7" r:id="rId4"/>
+    <sheet name="2x2 Update Calculator" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="98">
   <si>
     <t>Final</t>
   </si>
@@ -241,17 +242,90 @@
   <si>
     <t>Multivariate - Increasing b while trading</t>
   </si>
+  <si>
+    <t>Insurance Fraud</t>
+  </si>
+  <si>
+    <t>Assume unit price is 1$, insured facility worth $500.</t>
+  </si>
+  <si>
+    <t>Burn Down?</t>
+  </si>
+  <si>
+    <t>No-Fraud Actuarial Risk</t>
+  </si>
+  <si>
+    <t>Increments</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Ins Profit</t>
+  </si>
+  <si>
+    <t>Buyer</t>
+  </si>
+  <si>
+    <t>Seller</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Owner Cost</t>
+  </si>
+  <si>
+    <t>Note HIGH sensitivity to increments, particularly increments/value ratio</t>
+  </si>
+  <si>
+    <t>Ins</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Very interesting…converges to $20 (which is 4% * 500) only at high increments</t>
+  </si>
+  <si>
+    <t>capital tie up</t>
+  </si>
+  <si>
+    <t>problem</t>
+  </si>
+  <si>
+    <t>insurance strategy</t>
+  </si>
+  <si>
+    <t>augmentation</t>
+  </si>
+  <si>
+    <t>include price of arson</t>
+  </si>
+  <si>
+    <t>demand arson protections (or refuse to insure)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -861,7 +935,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1112,6 +1186,17 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1127,17 +1212,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1272,11 +1367,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="110977792"/>
-        <c:axId val="110979328"/>
+        <c:axId val="63996672"/>
+        <c:axId val="63998208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110977792"/>
+        <c:axId val="63996672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1285,7 +1380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110979328"/>
+        <c:crossAx val="63998208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1293,7 +1388,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110979328"/>
+        <c:axId val="63998208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1304,7 +1399,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110977792"/>
+        <c:crossAx val="63996672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1443,11 +1538,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113342720"/>
-        <c:axId val="113356800"/>
+        <c:axId val="65763584"/>
+        <c:axId val="65765376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113342720"/>
+        <c:axId val="65763584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1456,7 +1551,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113356800"/>
+        <c:crossAx val="65765376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1464,7 +1559,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113356800"/>
+        <c:axId val="65765376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1475,7 +1570,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113342720"/>
+        <c:crossAx val="65763584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2000,8 +2095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AP59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3655,7 +3750,7 @@
       <c r="AP7" s="7"/>
     </row>
     <row r="8" spans="2:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="183" t="s">
+      <c r="C8" s="178" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="136" t="s">
@@ -3721,7 +3816,7 @@
       <c r="B9" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="184">
+      <c r="C9" s="179">
         <v>2</v>
       </c>
       <c r="D9">
@@ -3795,7 +3890,7 @@
       <c r="B10" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="184">
+      <c r="C10" s="179">
         <v>2</v>
       </c>
       <c r="D10" s="7">
@@ -3868,7 +3963,7 @@
       <c r="B11" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="184">
+      <c r="C11" s="179">
         <v>2</v>
       </c>
       <c r="D11" s="17">
@@ -3912,11 +4007,11 @@
       </c>
       <c r="O11" s="7"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="181" t="s">
+      <c r="R11" s="176" t="s">
         <v>71</v>
       </c>
-      <c r="S11" s="182"/>
-      <c r="T11" s="182"/>
+      <c r="S11" s="177"/>
+      <c r="T11" s="177"/>
       <c r="U11" s="7"/>
       <c r="V11" s="30"/>
       <c r="W11" s="30"/>
@@ -3944,7 +4039,7 @@
       <c r="B12" s="164" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="185">
+      <c r="C12" s="180">
         <v>2</v>
       </c>
       <c r="D12" s="7">
@@ -4021,7 +4116,7 @@
       <c r="B13" s="164" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="185">
+      <c r="C13" s="180">
         <v>5</v>
       </c>
       <c r="D13" s="7">
@@ -4105,7 +4200,7 @@
       <c r="B14" s="164" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="185">
+      <c r="C14" s="180">
         <v>5</v>
       </c>
       <c r="D14" s="7">
@@ -4183,7 +4278,7 @@
       <c r="B15" s="164" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="185">
+      <c r="C15" s="180">
         <v>5</v>
       </c>
       <c r="D15" s="7">
@@ -4257,7 +4352,7 @@
       <c r="B16" s="164" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="185">
+      <c r="C16" s="180">
         <v>5</v>
       </c>
       <c r="D16" s="7">
@@ -4789,6 +4884,2225 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:T87"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="Q67" sqref="Q67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q5" s="196" t="s">
+        <v>7</v>
+      </c>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="D6" s="163"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6" s="135" t="s">
+        <v>77</v>
+      </c>
+      <c r="R6" s="7"/>
+      <c r="S6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="34">
+        <f>COUNTA(E11:F11)</f>
+        <v>2</v>
+      </c>
+      <c r="J7" s="34"/>
+      <c r="K7">
+        <f>I12</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="Q7" s="135"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="199">
+        <v>0.04</v>
+      </c>
+      <c r="T7" s="200">
+        <f>1-S7</f>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="135" t="s">
+        <v>79</v>
+      </c>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7">
+        <v>500</v>
+      </c>
+      <c r="T8" s="118"/>
+    </row>
+    <row r="9" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="7"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="Q9" s="143" t="s">
+        <v>78</v>
+      </c>
+      <c r="R9" s="198"/>
+      <c r="S9" s="198">
+        <v>5000</v>
+      </c>
+      <c r="T9" s="120"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="E10" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="69"/>
+      <c r="I10" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="69" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="20"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="20"/>
+    </row>
+    <row r="11" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="7"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="43">
+        <v>0</v>
+      </c>
+      <c r="J11" s="44"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+    </row>
+    <row r="12" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="45">
+        <v>0</v>
+      </c>
+      <c r="F12" s="46">
+        <v>0</v>
+      </c>
+      <c r="G12" s="51">
+        <f>EXP(E12/$T$5)/(EXP($F12/$T$5)+EXP($E12/$T$5))</f>
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="92">
+        <f>EXP(F12/$T$5)/(EXP($F12/$T$5)+EXP($E12/$T$5))</f>
+        <v>0.5</v>
+      </c>
+      <c r="I12" s="95">
+        <f>$T$5*LN(EXP($F12/$T$5)+EXP($E12/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J12" s="186">
+        <f>(I12-I11)</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" t="str">
+        <f>IF(D12="Buyer",J12,"")</f>
+        <v/>
+      </c>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="48">
+        <f>S8/S9</f>
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="42">
+        <v>0</v>
+      </c>
+      <c r="G13" s="49">
+        <f>EXP(E13/$T$5)/(EXP($F13/$T$5)+EXP($E13/$T$5))</f>
+        <v>0.52497918747894001</v>
+      </c>
+      <c r="H13" s="93">
+        <f>EXP(F13/$T$5)/(EXP($F13/$T$5)+EXP($E13/$T$5))</f>
+        <v>0.47502081252105999</v>
+      </c>
+      <c r="I13" s="96">
+        <f>$T$5*LN(EXP($F13/$T$5)+EXP($E13/$T$5))</f>
+        <v>0.74439666007357097</v>
+      </c>
+      <c r="J13" s="187">
+        <f>(I13-I12)</f>
+        <v>5.1249479513625684E-2</v>
+      </c>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="N13" s="201">
+        <f>IF(D13="Buyer",J13,"")</f>
+        <v>5.1249479513625684E-2</v>
+      </c>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="48">
+        <f>IF(MOD(ROW(A14),2)=1,E13+E12,E13)</f>
+        <v>0.1</v>
+      </c>
+      <c r="F14" s="191">
+        <f>IF(MOD(ROW(A14),2)=0,L14,F13)</f>
+        <v>3.2780538303479458</v>
+      </c>
+      <c r="G14" s="49">
+        <f>EXP(E14/$T$5)/(EXP($F14/$T$5)+EXP($E14/$T$5))</f>
+        <v>3.9999999999999994E-2</v>
+      </c>
+      <c r="H14" s="93">
+        <f>EXP(F14/$T$5)/(EXP($F14/$T$5)+EXP($E14/$T$5))</f>
+        <v>0.96000000000000008</v>
+      </c>
+      <c r="I14" s="96">
+        <f>$T$5*LN(EXP($F14/$T$5)+EXP($E14/$T$5))</f>
+        <v>3.3188758248682011</v>
+      </c>
+      <c r="J14" s="187">
+        <f>(I14-I13)</f>
+        <v>2.5744791647946301</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="144">
+        <f>$T$5*LN($T$7/$S$7)+E14</f>
+        <v>3.2780538303479458</v>
+      </c>
+      <c r="M14" s="144">
+        <f>IF( D14="Seller",((F14-F13)-J14)*$T$7,"")</f>
+        <v>0.67543167893118305</v>
+      </c>
+      <c r="N14" t="str">
+        <f>IF(D14="Buyer",J14,"")</f>
+        <v/>
+      </c>
+      <c r="P14" s="192"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="194"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="48">
+        <f>IF(MOD(ROW(A15),2)=1,E14+$E$13,E14)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F15" s="191">
+        <f>IF(MOD(ROW(A15),2)=0,L15,F14)</f>
+        <v>3.2780538303479458</v>
+      </c>
+      <c r="G15" s="49">
+        <f>EXP(E15/$T$5)/(EXP($F15/$T$5)+EXP($E15/$T$5))</f>
+        <v>4.4021644850859298E-2</v>
+      </c>
+      <c r="H15" s="93">
+        <f>EXP(F15/$T$5)/(EXP($F15/$T$5)+EXP($E15/$T$5))</f>
+        <v>0.95597835514914065</v>
+      </c>
+      <c r="I15" s="96">
+        <f>$T$5*LN(EXP($F15/$T$5)+EXP($E15/$T$5))</f>
+        <v>3.3230738375923785</v>
+      </c>
+      <c r="J15" s="187">
+        <f>(I15-I14)</f>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="K15" s="7"/>
+      <c r="L15" s="144">
+        <f>$T$5*LN($T$7/$S$7)+E15</f>
+        <v>3.3780538303479459</v>
+      </c>
+      <c r="M15" s="144" t="str">
+        <f t="shared" ref="M15:M30" si="0">IF( D15="Seller",((F15-F14)-J15)*$T$7,"")</f>
+        <v/>
+      </c>
+      <c r="N15">
+        <f>IF(D15="Buyer",J15,"")</f>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7">
+        <v>2</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="48">
+        <f t="shared" ref="E16:E29" si="1">IF(MOD(ROW(A16),2)=1,E15+$E$13,E15)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F16" s="191">
+        <f>IF(MOD(ROW(A16),2)=0,L16,F15)</f>
+        <v>3.3780538303479459</v>
+      </c>
+      <c r="G16" s="49">
+        <f t="shared" ref="G16:G30" si="2">EXP(E16/$T$5)/(EXP($F16/$T$5)+EXP($E16/$T$5))</f>
+        <v>3.9999999999999987E-2</v>
+      </c>
+      <c r="H16" s="93">
+        <f t="shared" ref="H16:H30" si="3">EXP(F16/$T$5)/(EXP($F16/$T$5)+EXP($E16/$T$5))</f>
+        <v>0.96</v>
+      </c>
+      <c r="I16" s="96">
+        <f>$T$5*LN(EXP($F16/$T$5)+EXP($E16/$T$5))</f>
+        <v>3.4188758248682012</v>
+      </c>
+      <c r="J16" s="187">
+        <f t="shared" ref="J15:J30" si="4">(I16-I15)</f>
+        <v>9.5801987275822675E-2</v>
+      </c>
+      <c r="K16" s="7"/>
+      <c r="L16" s="144">
+        <f t="shared" ref="L16:L29" si="5">$T$5*LN($T$7/$S$7)+E16</f>
+        <v>3.3780538303479459</v>
+      </c>
+      <c r="M16" s="144">
+        <f>IF( D16="Seller",((F16-F15)-J16)*$T$7,"")</f>
+        <v>4.0300922152103165E-3</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" ref="N13:N30" si="6">IF(D16="Buyer",J16,"")</f>
+        <v/>
+      </c>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="D17" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="48">
+        <f t="shared" si="1"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="F17" s="191">
+        <f t="shared" ref="F15:F27" si="7">IF(MOD(ROW(A17),2)=0,L17,F16)</f>
+        <v>3.3780538303479459</v>
+      </c>
+      <c r="G17" s="49">
+        <f t="shared" si="2"/>
+        <v>4.4021644850859298E-2</v>
+      </c>
+      <c r="H17" s="93">
+        <f t="shared" si="3"/>
+        <v>0.95597835514914076</v>
+      </c>
+      <c r="I17" s="96">
+        <f>$T$5*LN(EXP($F17/$T$5)+EXP($E17/$T$5))</f>
+        <v>3.4230738375923786</v>
+      </c>
+      <c r="J17" s="187">
+        <f t="shared" si="4"/>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="K17" s="7"/>
+      <c r="L17" s="144">
+        <f t="shared" si="5"/>
+        <v>3.478053830347946</v>
+      </c>
+      <c r="M17" s="144" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N17">
+        <f t="shared" si="6"/>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="48">
+        <f t="shared" si="1"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="F18" s="191">
+        <f t="shared" si="7"/>
+        <v>3.478053830347946</v>
+      </c>
+      <c r="G18" s="49">
+        <f t="shared" si="2"/>
+        <v>3.9999999999999987E-2</v>
+      </c>
+      <c r="H18" s="93">
+        <f t="shared" si="3"/>
+        <v>0.96</v>
+      </c>
+      <c r="I18" s="96">
+        <f>$T$5*LN(EXP($F18/$T$5)+EXP($E18/$T$5))</f>
+        <v>3.5188758248682013</v>
+      </c>
+      <c r="J18" s="187">
+        <f t="shared" si="4"/>
+        <v>9.5801987275822675E-2</v>
+      </c>
+      <c r="K18" s="7"/>
+      <c r="L18" s="144">
+        <f t="shared" si="5"/>
+        <v>3.478053830347946</v>
+      </c>
+      <c r="M18" s="144">
+        <f>IF( D18="Seller",((F18-F17)-J18)*$T$7,"")</f>
+        <v>4.0300922152103165E-3</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="48">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="F19" s="191">
+        <f t="shared" si="7"/>
+        <v>3.478053830347946</v>
+      </c>
+      <c r="G19" s="49">
+        <f t="shared" si="2"/>
+        <v>4.4021644850859291E-2</v>
+      </c>
+      <c r="H19" s="93">
+        <f t="shared" si="3"/>
+        <v>0.95597835514914076</v>
+      </c>
+      <c r="I19" s="96">
+        <f>$T$5*LN(EXP($F19/$T$5)+EXP($E19/$T$5))</f>
+        <v>3.5230738375923787</v>
+      </c>
+      <c r="J19" s="187">
+        <f t="shared" si="4"/>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="K19" s="7"/>
+      <c r="L19" s="144">
+        <f t="shared" si="5"/>
+        <v>3.5780538303479457</v>
+      </c>
+      <c r="M19" s="144" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N19">
+        <f t="shared" si="6"/>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7">
+        <v>4</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="48">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="F20" s="191">
+        <f t="shared" si="7"/>
+        <v>3.5780538303479457</v>
+      </c>
+      <c r="G20" s="49">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+      <c r="H20" s="93">
+        <f t="shared" si="3"/>
+        <v>0.96</v>
+      </c>
+      <c r="I20" s="96">
+        <f>$T$5*LN(EXP($F20/$T$5)+EXP($E20/$T$5))</f>
+        <v>3.6188758248682009</v>
+      </c>
+      <c r="J20" s="187">
+        <f t="shared" si="4"/>
+        <v>9.5801987275822231E-2</v>
+      </c>
+      <c r="K20" s="7"/>
+      <c r="L20" s="144">
+        <f t="shared" si="5"/>
+        <v>3.5780538303479457</v>
+      </c>
+      <c r="M20" s="144">
+        <f>IF( D20="Seller",((F20-F19)-J20)*$T$7,"")</f>
+        <v>4.0300922152103165E-3</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="48">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="191">
+        <f t="shared" ref="F21:F29" si="8">IF(MOD(ROW(A21),2)=0,L21,F20)</f>
+        <v>3.5780538303479457</v>
+      </c>
+      <c r="G21" s="49">
+        <f t="shared" si="2"/>
+        <v>4.4021644850859305E-2</v>
+      </c>
+      <c r="H21" s="93">
+        <f t="shared" si="3"/>
+        <v>0.95597835514914065</v>
+      </c>
+      <c r="I21" s="96">
+        <f>$T$5*LN(EXP($F21/$T$5)+EXP($E21/$T$5))</f>
+        <v>3.6230738375923783</v>
+      </c>
+      <c r="J21" s="187">
+        <f t="shared" si="4"/>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="K21" s="7"/>
+      <c r="L21" s="144">
+        <f t="shared" si="5"/>
+        <v>3.6780538303479458</v>
+      </c>
+      <c r="M21" s="144" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N21">
+        <f t="shared" si="6"/>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7">
+        <v>5</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="48">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="F22" s="191">
+        <f t="shared" si="8"/>
+        <v>3.6780538303479458</v>
+      </c>
+      <c r="G22" s="49">
+        <f t="shared" si="2"/>
+        <v>3.9999999999999994E-2</v>
+      </c>
+      <c r="H22" s="93">
+        <f t="shared" si="3"/>
+        <v>0.96</v>
+      </c>
+      <c r="I22" s="96">
+        <f>$T$5*LN(EXP($F22/$T$5)+EXP($E22/$T$5))</f>
+        <v>3.718875824868201</v>
+      </c>
+      <c r="J22" s="187">
+        <f>(I22-I21)</f>
+        <v>9.5801987275822675E-2</v>
+      </c>
+      <c r="K22" s="7"/>
+      <c r="L22" s="144">
+        <f>$T$5*LN($T$7/$S$7)+E22</f>
+        <v>3.6780538303479458</v>
+      </c>
+      <c r="M22" s="144">
+        <f t="shared" si="0"/>
+        <v>4.0300922152103165E-3</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="48">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="F23" s="191">
+        <f t="shared" si="8"/>
+        <v>3.6780538303479458</v>
+      </c>
+      <c r="G23" s="49">
+        <f t="shared" si="2"/>
+        <v>4.4021644850859298E-2</v>
+      </c>
+      <c r="H23" s="93">
+        <f t="shared" si="3"/>
+        <v>0.95597835514914076</v>
+      </c>
+      <c r="I23" s="96">
+        <f>$T$5*LN(EXP($F23/$T$5)+EXP($E23/$T$5))</f>
+        <v>3.7230738375923784</v>
+      </c>
+      <c r="J23" s="187">
+        <f t="shared" si="4"/>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="K23" s="7"/>
+      <c r="L23" s="144">
+        <f t="shared" si="5"/>
+        <v>3.7780538303479458</v>
+      </c>
+      <c r="M23" s="144" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N23">
+        <f>IF(D23="Buyer",J23,"")</f>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="48">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="F24" s="191">
+        <f t="shared" si="8"/>
+        <v>3.7780538303479458</v>
+      </c>
+      <c r="G24" s="49">
+        <f t="shared" si="2"/>
+        <v>3.9999999999999994E-2</v>
+      </c>
+      <c r="H24" s="93">
+        <f t="shared" si="3"/>
+        <v>0.96000000000000008</v>
+      </c>
+      <c r="I24" s="96">
+        <f>$T$5*LN(EXP($F24/$T$5)+EXP($E24/$T$5))</f>
+        <v>3.8188758248682011</v>
+      </c>
+      <c r="J24" s="187">
+        <f t="shared" si="4"/>
+        <v>9.5801987275822675E-2</v>
+      </c>
+      <c r="K24" s="7"/>
+      <c r="L24" s="144">
+        <f t="shared" si="5"/>
+        <v>3.7780538303479458</v>
+      </c>
+      <c r="M24" s="144">
+        <f t="shared" si="0"/>
+        <v>4.0300922152103165E-3</v>
+      </c>
+      <c r="N24" t="str">
+        <f>IF(D24="Buyer",J24,"")</f>
+        <v/>
+      </c>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="48">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="F25" s="191">
+        <f t="shared" si="8"/>
+        <v>3.7780538303479458</v>
+      </c>
+      <c r="G25" s="49">
+        <f t="shared" si="2"/>
+        <v>4.4021644850859298E-2</v>
+      </c>
+      <c r="H25" s="93">
+        <f t="shared" si="3"/>
+        <v>0.95597835514914076</v>
+      </c>
+      <c r="I25" s="96">
+        <f>$T$5*LN(EXP($F25/$T$5)+EXP($E25/$T$5))</f>
+        <v>3.8230738375923785</v>
+      </c>
+      <c r="J25" s="187">
+        <f t="shared" si="4"/>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="K25" s="7"/>
+      <c r="L25" s="144">
+        <f t="shared" si="5"/>
+        <v>3.8780538303479455</v>
+      </c>
+      <c r="M25" s="144" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N25">
+        <f t="shared" si="6"/>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7">
+        <v>7</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="48">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="F26" s="191">
+        <f t="shared" si="8"/>
+        <v>3.8780538303479455</v>
+      </c>
+      <c r="G26" s="49">
+        <f t="shared" si="2"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="H26" s="93">
+        <f t="shared" si="3"/>
+        <v>0.96000000000000008</v>
+      </c>
+      <c r="I26" s="96">
+        <f>$T$5*LN(EXP($F26/$T$5)+EXP($E26/$T$5))</f>
+        <v>3.9188758248682007</v>
+      </c>
+      <c r="J26" s="187">
+        <f>(I26-I25)</f>
+        <v>9.5801987275822231E-2</v>
+      </c>
+      <c r="K26" s="7"/>
+      <c r="L26" s="144">
+        <f t="shared" si="5"/>
+        <v>3.8780538303479455</v>
+      </c>
+      <c r="M26" s="144">
+        <f t="shared" si="0"/>
+        <v>4.0300922152103165E-3</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="48">
+        <f t="shared" si="1"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="F27" s="191">
+        <f t="shared" si="8"/>
+        <v>3.8780538303479455</v>
+      </c>
+      <c r="G27" s="49">
+        <f t="shared" si="2"/>
+        <v>4.4021644850859305E-2</v>
+      </c>
+      <c r="H27" s="93">
+        <f t="shared" si="3"/>
+        <v>0.95597835514914065</v>
+      </c>
+      <c r="I27" s="96">
+        <f>$T$5*LN(EXP($F27/$T$5)+EXP($E27/$T$5))</f>
+        <v>3.9230738375923782</v>
+      </c>
+      <c r="J27" s="187">
+        <f t="shared" si="4"/>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="K27" s="7"/>
+      <c r="L27" s="144">
+        <f t="shared" si="5"/>
+        <v>3.9780538303479456</v>
+      </c>
+      <c r="M27" s="144" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N27">
+        <f t="shared" si="6"/>
+        <v>4.1980127241774134E-3</v>
+      </c>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7">
+        <v>8</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="48">
+        <f t="shared" si="1"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="F28" s="191">
+        <f t="shared" si="8"/>
+        <v>3.9780538303479456</v>
+      </c>
+      <c r="G28" s="49">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+      <c r="H28" s="93">
+        <f t="shared" si="3"/>
+        <v>0.96000000000000008</v>
+      </c>
+      <c r="I28" s="96">
+        <f>$T$5*LN(EXP($F28/$T$5)+EXP($E28/$T$5))</f>
+        <v>4.0188758248682008</v>
+      </c>
+      <c r="J28" s="187">
+        <f t="shared" si="4"/>
+        <v>9.5801987275822675E-2</v>
+      </c>
+      <c r="K28" s="7"/>
+      <c r="L28" s="144">
+        <f t="shared" si="5"/>
+        <v>3.9780538303479456</v>
+      </c>
+      <c r="M28" s="144">
+        <f>IF( D28="Seller",((F28-F27)-J28)*$T$7,"")</f>
+        <v>4.0300922152103165E-3</v>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+      <c r="D29" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="48">
+        <f t="shared" si="1"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="F29" s="191">
+        <f t="shared" si="8"/>
+        <v>3.9780538303479456</v>
+      </c>
+      <c r="G29" s="49">
+        <f t="shared" si="2"/>
+        <v>4.4021644850859305E-2</v>
+      </c>
+      <c r="H29" s="93">
+        <f t="shared" si="3"/>
+        <v>0.95597835514914065</v>
+      </c>
+      <c r="I29" s="96">
+        <f>$T$5*LN(EXP($F29/$T$5)+EXP($E29/$T$5))</f>
+        <v>4.0230738375923778</v>
+      </c>
+      <c r="J29" s="187">
+        <f t="shared" si="4"/>
+        <v>4.1980127241769694E-3</v>
+      </c>
+      <c r="K29" s="7"/>
+      <c r="L29" s="144">
+        <f t="shared" si="5"/>
+        <v>4.0780538303479457</v>
+      </c>
+      <c r="M29" s="144" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+    </row>
+    <row r="30" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="48">
+        <v>0</v>
+      </c>
+      <c r="F30" s="193">
+        <f t="shared" ref="F17:F30" si="9">F29</f>
+        <v>3.9780538303479456</v>
+      </c>
+      <c r="G30" s="49">
+        <f t="shared" si="2"/>
+        <v>1.8377967132622502E-2</v>
+      </c>
+      <c r="H30" s="93">
+        <f t="shared" si="3"/>
+        <v>0.98162203286737748</v>
+      </c>
+      <c r="I30" s="133">
+        <f>$T$5*LN(EXP($F30/$T$5)+EXP($E30/$T$5))</f>
+        <v>3.9966027703138742</v>
+      </c>
+      <c r="J30" s="188">
+        <f t="shared" si="4"/>
+        <v>-2.6471067278503568E-2</v>
+      </c>
+      <c r="K30" s="7"/>
+      <c r="L30" s="144">
+        <f>$T$5*LN($T$7/$S$7)+E30</f>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M30" s="144" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+    </row>
+    <row r="31" spans="2:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="52">
+        <f>E30</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="195">
+        <f>F30</f>
+        <v>3.9780538303479456</v>
+      </c>
+      <c r="G31" s="54">
+        <f>EXP(E31)/(EXP($F31)+EXP($E31))</f>
+        <v>1.8377967132622502E-2</v>
+      </c>
+      <c r="H31" s="94">
+        <f>EXP(F31)/(EXP($F31)+EXP($E31))</f>
+        <v>0.98162203286737748</v>
+      </c>
+      <c r="I31" s="97">
+        <f>$T$5*LN(EXP($F31/$T$5)+EXP($E31/$T$5))</f>
+        <v>3.9966027703138742</v>
+      </c>
+      <c r="J31" s="189">
+        <f>SUM(J12:J30)</f>
+        <v>3.9966027703138742</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="8"/>
+    </row>
+    <row r="32" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="7"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="130">
+        <v>0</v>
+      </c>
+      <c r="J32" s="190">
+        <f>J31-(SUMPRODUCT(G31:H31,E31:F31))</f>
+        <v>9.1657482511866117E-2</v>
+      </c>
+      <c r="K32" t="s">
+        <v>64</v>
+      </c>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+    </row>
+    <row r="34" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>87</v>
+      </c>
+      <c r="N34" t="s">
+        <v>88</v>
+      </c>
+      <c r="O34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <f>M14+(M28*($S$9-1))</f>
+        <v>20.821862662767554</v>
+      </c>
+      <c r="N35">
+        <f>N13+(N27*($S$9-1))</f>
+        <v>21.037115087676515</v>
+      </c>
+      <c r="O35">
+        <f>K7</f>
+        <v>0.69314718055994529</v>
+      </c>
+    </row>
+    <row r="37" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>92</v>
+      </c>
+      <c r="J37">
+        <f>(J26*S9)+J14</f>
+        <v>481.58441554390578</v>
+      </c>
+      <c r="M37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <f>S7*S8</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q52" s="196" t="s">
+        <v>7</v>
+      </c>
+      <c r="R52" s="10"/>
+      <c r="S52" s="10"/>
+      <c r="T52" s="197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="3:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="D53" s="163"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="34"/>
+      <c r="K53" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q53" s="135" t="s">
+        <v>77</v>
+      </c>
+      <c r="R53" s="7"/>
+      <c r="S53" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="T53" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>76</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F54" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G54" s="34"/>
+      <c r="H54" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="I54" s="34">
+        <f>COUNTA(E58:F58)</f>
+        <v>2</v>
+      </c>
+      <c r="J54" s="34"/>
+      <c r="K54">
+        <f>I59</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="Q54" s="135"/>
+      <c r="R54" s="7"/>
+      <c r="S54" s="199">
+        <v>0.04</v>
+      </c>
+      <c r="T54" s="200">
+        <f>1-S54</f>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="55" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D55" s="7"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="34"/>
+      <c r="H55" s="34"/>
+      <c r="I55" s="34"/>
+      <c r="J55" s="34"/>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="135" t="s">
+        <v>79</v>
+      </c>
+      <c r="R55" s="7"/>
+      <c r="S55" s="7">
+        <v>500</v>
+      </c>
+      <c r="T55" s="118"/>
+    </row>
+    <row r="56" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="34"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="34"/>
+      <c r="J56" s="34"/>
+      <c r="Q56" s="143" t="s">
+        <v>78</v>
+      </c>
+      <c r="R56" s="198"/>
+      <c r="S56" s="198">
+        <v>5000</v>
+      </c>
+      <c r="T56" s="120"/>
+    </row>
+    <row r="57" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="E57" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="F57" s="68"/>
+      <c r="G57" s="68" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" s="69"/>
+      <c r="I57" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="J57" s="69" t="s">
+        <v>37</v>
+      </c>
+      <c r="K57" s="20"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="7"/>
+      <c r="P57" s="7"/>
+      <c r="Q57" s="20"/>
+    </row>
+    <row r="58" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D58" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E58" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="H58" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="I58" s="43">
+        <v>0</v>
+      </c>
+      <c r="J58" s="44"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
+      <c r="N58" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O58" s="7"/>
+      <c r="P58" s="7"/>
+      <c r="Q58" s="202"/>
+    </row>
+    <row r="59" spans="3:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D59" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E59" s="45">
+        <v>0</v>
+      </c>
+      <c r="F59" s="46">
+        <v>0</v>
+      </c>
+      <c r="G59" s="51">
+        <f>EXP(E59/$T$5)/(EXP($F59/$T$5)+EXP($E59/$T$5))</f>
+        <v>0.5</v>
+      </c>
+      <c r="H59" s="92">
+        <f>EXP(F59/$T$5)/(EXP($F59/$T$5)+EXP($E59/$T$5))</f>
+        <v>0.5</v>
+      </c>
+      <c r="I59" s="95">
+        <f>$T$5*LN(EXP($F59/$T$5)+EXP($E59/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J59" s="186">
+        <f>(I59-I58)</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" t="str">
+        <f>IF(D59="Buyer",J59,"")</f>
+        <v/>
+      </c>
+      <c r="P59" s="7"/>
+      <c r="Q59" s="7"/>
+    </row>
+    <row r="60" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D60" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E60" s="48">
+        <v>500</v>
+      </c>
+      <c r="F60" s="42">
+        <v>503.18</v>
+      </c>
+      <c r="G60" s="49">
+        <f>EXP(E60/$T$5)/(EXP($F60/$T$5)+EXP($E60/$T$5))</f>
+        <v>3.992533395281353E-2</v>
+      </c>
+      <c r="H60" s="93">
+        <f>EXP(F60/$T$5)/(EXP($F60/$T$5)+EXP($E60/$T$5))</f>
+        <v>0.96007466604718639</v>
+      </c>
+      <c r="I60" s="96">
+        <f>$T$5*LN(EXP($F60/$T$5)+EXP($E60/$T$5))</f>
+        <v>503.22074422041226</v>
+      </c>
+      <c r="J60" s="187">
+        <f>(I60-I59)</f>
+        <v>502.52759703985231</v>
+      </c>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M60" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="N60" s="201">
+        <f>IF(D60="Buyer",J60,"")</f>
+        <v>502.52759703985231</v>
+      </c>
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7"/>
+    </row>
+    <row r="61" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D61" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E61" s="48">
+        <f>IF(MOD(ROW(A61),2)=1,E60+E59,E60)</f>
+        <v>500</v>
+      </c>
+      <c r="F61" s="42">
+        <v>503.18</v>
+      </c>
+      <c r="G61" s="49">
+        <f>EXP(E61/$T$5)/(EXP($F61/$T$5)+EXP($E61/$T$5))</f>
+        <v>3.992533395281353E-2</v>
+      </c>
+      <c r="H61" s="93">
+        <f>EXP(F61/$T$5)/(EXP($F61/$T$5)+EXP($E61/$T$5))</f>
+        <v>0.96007466604718639</v>
+      </c>
+      <c r="I61" s="96">
+        <f>$T$5*LN(EXP($F61/$T$5)+EXP($E61/$T$5))</f>
+        <v>503.22074422041226</v>
+      </c>
+      <c r="J61" s="187">
+        <f>(I61-I60)</f>
+        <v>0</v>
+      </c>
+      <c r="K61" s="7"/>
+      <c r="L61" s="144">
+        <f>$T$5*LN($T$7/$S$7)+E61</f>
+        <v>503.17805383034795</v>
+      </c>
+      <c r="M61" s="144">
+        <f>IF( D61="Seller",((F61-F60)-J61)*$T$7,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N61" t="str">
+        <f>IF(D61="Buyer",J61,"")</f>
+        <v/>
+      </c>
+      <c r="P61" s="192"/>
+      <c r="Q61" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="R61" s="194"/>
+    </row>
+    <row r="62" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>93</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E62" s="48">
+        <v>510</v>
+      </c>
+      <c r="F62" s="191">
+        <f>F61</f>
+        <v>503.18</v>
+      </c>
+      <c r="G62" s="49">
+        <f>EXP(E62/$T$5)/(EXP($F62/$T$5)+EXP($E62/$T$5))</f>
+        <v>0.99890946963253902</v>
+      </c>
+      <c r="H62" s="93">
+        <f>EXP(F62/$T$5)/(EXP($F62/$T$5)+EXP($E62/$T$5))</f>
+        <v>1.0905303674609804E-3</v>
+      </c>
+      <c r="I62" s="96">
+        <f>$T$5*LN(EXP($F62/$T$5)+EXP($E62/$T$5))</f>
+        <v>510.00109112542839</v>
+      </c>
+      <c r="J62" s="187">
+        <f t="shared" ref="J62:J77" si="10">(I62-I61)</f>
+        <v>6.7803469050161311</v>
+      </c>
+      <c r="K62" s="7"/>
+      <c r="L62" s="144">
+        <f>$T$5*LN($T$7/$S$7)+E62</f>
+        <v>513.17805383034795</v>
+      </c>
+      <c r="M62" s="144" t="str">
+        <f t="shared" ref="M62:M77" si="11">IF( D62="Seller",((F62-F61)-J62)*$T$7,"")</f>
+        <v/>
+      </c>
+      <c r="N62">
+        <f>IF(D62="Buyer",J62,"")</f>
+        <v>6.7803469050161311</v>
+      </c>
+      <c r="P62" s="7"/>
+      <c r="Q62" s="7"/>
+    </row>
+    <row r="63" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D63" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E63" s="48">
+        <v>510</v>
+      </c>
+      <c r="F63" s="191">
+        <v>0</v>
+      </c>
+      <c r="G63" s="49">
+        <f t="shared" ref="G63:G77" si="12">EXP(E63/$T$5)/(EXP($F63/$T$5)+EXP($E63/$T$5))</f>
+        <v>1</v>
+      </c>
+      <c r="H63" s="93">
+        <f t="shared" ref="H63:H77" si="13">EXP(F63/$T$5)/(EXP($F63/$T$5)+EXP($E63/$T$5))</f>
+        <v>3.2345526845351109E-222</v>
+      </c>
+      <c r="I63" s="96">
+        <f>$T$5*LN(EXP($F63/$T$5)+EXP($E63/$T$5))</f>
+        <v>510</v>
+      </c>
+      <c r="J63" s="187">
+        <f>(I63-I62)</f>
+        <v>-1.0911254283882954E-3</v>
+      </c>
+      <c r="K63" s="7"/>
+      <c r="L63" s="144">
+        <f t="shared" ref="L63:L76" si="14">$T$5*LN($T$7/$S$7)+E63</f>
+        <v>513.17805383034795</v>
+      </c>
+      <c r="M63" s="144">
+        <f>IF( D63="Seller",((F63-F62)-J63)*$T$7,"")</f>
+        <v>-483.05175251958872</v>
+      </c>
+      <c r="N63" t="str">
+        <f t="shared" ref="N63:N80" si="15">IF(D63="Buyer",J63,"")</f>
+        <v/>
+      </c>
+      <c r="O63" s="7"/>
+      <c r="P63" s="7"/>
+      <c r="Q63" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D64" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E64" s="48"/>
+      <c r="F64" s="191"/>
+      <c r="G64" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H64" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I64" s="96">
+        <f>$T$5*LN(EXP($F64/$T$5)+EXP($E64/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J64" s="187">
+        <f t="shared" si="10"/>
+        <v>-509.30685281944005</v>
+      </c>
+      <c r="K64" s="7"/>
+      <c r="L64" s="144">
+        <f t="shared" si="14"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M64" s="144" t="str">
+        <f t="shared" ref="M64:M79" si="16">IF( D64="Seller",((F64-F63)-J64)*$T$7,"")</f>
+        <v/>
+      </c>
+      <c r="N64">
+        <f t="shared" si="15"/>
+        <v>-509.30685281944005</v>
+      </c>
+      <c r="O64" s="7"/>
+      <c r="P64" s="7"/>
+      <c r="Q64" s="7"/>
+    </row>
+    <row r="65" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D65" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E65" s="48"/>
+      <c r="F65" s="191"/>
+      <c r="G65" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H65" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I65" s="96">
+        <f>$T$5*LN(EXP($F65/$T$5)+EXP($E65/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J65" s="187">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K65" s="7"/>
+      <c r="L65" s="144">
+        <f t="shared" si="14"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M65" s="144">
+        <f>IF( D65="Seller",((F65-F64)-J65)*$T$7,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N65" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O65" s="7"/>
+      <c r="P65" s="7"/>
+      <c r="Q65" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D66" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E66" s="48"/>
+      <c r="F66" s="191"/>
+      <c r="G66" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H66" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I66" s="96">
+        <f>$T$5*LN(EXP($F66/$T$5)+EXP($E66/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J66" s="187">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K66" s="7"/>
+      <c r="L66" s="144">
+        <f t="shared" si="14"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M66" s="144" t="str">
+        <f t="shared" ref="M66:M81" si="17">IF( D66="Seller",((F66-F65)-J66)*$T$7,"")</f>
+        <v/>
+      </c>
+      <c r="N66">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="O66" s="7"/>
+      <c r="P66" s="7"/>
+      <c r="Q66" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D67" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E67" s="48"/>
+      <c r="F67" s="191"/>
+      <c r="G67" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H67" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I67" s="96">
+        <f>$T$5*LN(EXP($F67/$T$5)+EXP($E67/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J67" s="187">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K67" s="7"/>
+      <c r="L67" s="144">
+        <f t="shared" si="14"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M67" s="144">
+        <f>IF( D67="Seller",((F67-F66)-J67)*$T$7,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N67" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O67" s="7"/>
+      <c r="P67" s="7"/>
+      <c r="Q67" s="7"/>
+    </row>
+    <row r="68" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D68" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E68" s="48"/>
+      <c r="F68" s="191"/>
+      <c r="G68" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H68" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I68" s="96">
+        <f>$T$5*LN(EXP($F68/$T$5)+EXP($E68/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J68" s="187">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K68" s="7"/>
+      <c r="L68" s="144">
+        <f t="shared" si="14"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M68" s="144" t="str">
+        <f t="shared" ref="M68:M83" si="18">IF( D68="Seller",((F68-F67)-J68)*$T$7,"")</f>
+        <v/>
+      </c>
+      <c r="N68">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="O68" s="7"/>
+      <c r="P68" s="7"/>
+      <c r="Q68" s="7"/>
+    </row>
+    <row r="69" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D69" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E69" s="48"/>
+      <c r="F69" s="191"/>
+      <c r="G69" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H69" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I69" s="96">
+        <f>$T$5*LN(EXP($F69/$T$5)+EXP($E69/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J69" s="187">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K69" s="7"/>
+      <c r="L69" s="144">
+        <f t="shared" si="14"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M69" s="144">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="N69" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O69" s="7"/>
+      <c r="P69" s="7"/>
+      <c r="Q69" s="7"/>
+    </row>
+    <row r="70" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D70" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E70" s="48"/>
+      <c r="F70" s="191"/>
+      <c r="G70" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H70" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I70" s="96">
+        <f>$T$5*LN(EXP($F70/$T$5)+EXP($E70/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J70" s="187">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K70" s="7"/>
+      <c r="L70" s="144">
+        <f t="shared" si="14"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M70" s="144" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="N70">
+        <f>IF(D70="Buyer",J70,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O70" s="7"/>
+      <c r="P70" s="7"/>
+      <c r="Q70" s="7"/>
+    </row>
+    <row r="71" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D71" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E71" s="48"/>
+      <c r="F71" s="191"/>
+      <c r="G71" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H71" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I71" s="96">
+        <f>$T$5*LN(EXP($F71/$T$5)+EXP($E71/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J71" s="187">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K71" s="7"/>
+      <c r="L71" s="144">
+        <f t="shared" si="14"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M71" s="144">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="N71" t="str">
+        <f>IF(D71="Buyer",J71,"")</f>
+        <v/>
+      </c>
+      <c r="O71" s="7"/>
+      <c r="P71" s="7"/>
+      <c r="Q71" s="7"/>
+    </row>
+    <row r="72" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D72" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E72" s="48"/>
+      <c r="F72" s="191"/>
+      <c r="G72" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H72" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I72" s="96">
+        <f>$T$5*LN(EXP($F72/$T$5)+EXP($E72/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J72" s="187">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K72" s="7"/>
+      <c r="L72" s="144">
+        <f t="shared" si="14"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M72" s="144" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="N72">
+        <f t="shared" ref="N72:N88" si="19">IF(D72="Buyer",J72,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O72" s="7"/>
+      <c r="P72" s="7"/>
+      <c r="Q72" s="7"/>
+    </row>
+    <row r="73" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D73" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E73" s="48"/>
+      <c r="F73" s="191"/>
+      <c r="G73" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H73" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I73" s="96">
+        <f>$T$5*LN(EXP($F73/$T$5)+EXP($E73/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J73" s="187">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K73" s="7"/>
+      <c r="L73" s="144">
+        <f t="shared" si="14"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M73" s="144">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="N73" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="O73" s="7"/>
+      <c r="P73" s="7"/>
+      <c r="Q73" s="7"/>
+    </row>
+    <row r="74" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D74" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E74" s="48"/>
+      <c r="F74" s="191"/>
+      <c r="G74" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H74" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I74" s="96">
+        <f>$T$5*LN(EXP($F74/$T$5)+EXP($E74/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J74" s="187">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K74" s="7"/>
+      <c r="L74" s="144">
+        <f t="shared" si="14"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M74" s="144" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="N74">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O74" s="7"/>
+      <c r="P74" s="7"/>
+      <c r="Q74" s="7"/>
+    </row>
+    <row r="75" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D75" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E75" s="48"/>
+      <c r="F75" s="191"/>
+      <c r="G75" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H75" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I75" s="96">
+        <f>$T$5*LN(EXP($F75/$T$5)+EXP($E75/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J75" s="187">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K75" s="7"/>
+      <c r="L75" s="144">
+        <f t="shared" si="14"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M75" s="144">
+        <f>IF( D75="Seller",((F75-F74)-J75)*$T$7,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N75" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="O75" s="7"/>
+      <c r="P75" s="7"/>
+      <c r="Q75" s="7"/>
+    </row>
+    <row r="76" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D76" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E76" s="48"/>
+      <c r="F76" s="191"/>
+      <c r="G76" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H76" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I76" s="96">
+        <f>$T$5*LN(EXP($F76/$T$5)+EXP($E76/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J76" s="187">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K76" s="7"/>
+      <c r="L76" s="144">
+        <f t="shared" si="14"/>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M76" s="144" t="str">
+        <f t="shared" ref="M76:M88" si="20">IF( D76="Seller",((F76-F75)-J76)*$T$7,"")</f>
+        <v/>
+      </c>
+      <c r="N76" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="O76" s="7"/>
+      <c r="P76" s="7"/>
+      <c r="Q76" s="7"/>
+    </row>
+    <row r="77" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D77" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E77" s="48"/>
+      <c r="F77" s="193"/>
+      <c r="G77" s="49">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="H77" s="93">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I77" s="133">
+        <f>$T$5*LN(EXP($F77/$T$5)+EXP($E77/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J77" s="188">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K77" s="7"/>
+      <c r="L77" s="144">
+        <f>$T$5*LN($T$7/$S$7)+E77</f>
+        <v>3.1780538303479458</v>
+      </c>
+      <c r="M77" s="144" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="N77" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="O77" s="7"/>
+      <c r="P77" s="7"/>
+      <c r="Q77" s="7"/>
+    </row>
+    <row r="78" spans="4:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D78" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="52">
+        <f>E77</f>
+        <v>0</v>
+      </c>
+      <c r="F78" s="195">
+        <f>F77</f>
+        <v>0</v>
+      </c>
+      <c r="G78" s="54">
+        <f>EXP(E78)/(EXP($F78)+EXP($E78))</f>
+        <v>0.5</v>
+      </c>
+      <c r="H78" s="94">
+        <f>EXP(F78)/(EXP($F78)+EXP($E78))</f>
+        <v>0.5</v>
+      </c>
+      <c r="I78" s="97">
+        <f>$T$5*LN(EXP($F78/$T$5)+EXP($E78/$T$5))</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="J78" s="189">
+        <f>SUM(J59:J77)</f>
+        <v>0.69314718055994717</v>
+      </c>
+      <c r="K78" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L78" s="7"/>
+      <c r="M78" s="7"/>
+      <c r="N78" s="7"/>
+      <c r="O78" s="7"/>
+      <c r="P78" s="7"/>
+      <c r="Q78" s="8"/>
+    </row>
+    <row r="79" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E79" s="34"/>
+      <c r="F79" s="34"/>
+      <c r="G79" s="34"/>
+      <c r="H79" s="34"/>
+      <c r="I79" s="130">
+        <v>0</v>
+      </c>
+      <c r="J79" s="190">
+        <f>J78-(SUMPRODUCT(G78:H78,E78:F78))</f>
+        <v>0.69314718055994717</v>
+      </c>
+      <c r="K79" t="s">
+        <v>64</v>
+      </c>
+      <c r="L79" s="7"/>
+      <c r="M79" s="7"/>
+      <c r="N79" s="7"/>
+      <c r="O79" s="7"/>
+      <c r="P79" s="7"/>
+    </row>
+    <row r="81" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M81" t="s">
+        <v>87</v>
+      </c>
+      <c r="N81" t="s">
+        <v>88</v>
+      </c>
+      <c r="O81" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M82">
+        <f>M61+(M75*($S$9-1))</f>
+        <v>0</v>
+      </c>
+      <c r="N82">
+        <f>N60+(N74*($S$9-1))</f>
+        <v>502.52759703985231</v>
+      </c>
+      <c r="O82">
+        <f>K54</f>
+        <v>0.69314718055994529</v>
+      </c>
+    </row>
+    <row r="84" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M84" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M86" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="87" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="N87">
+        <f>S54*S55</f>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7710,7 +10024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U22"/>
   <sheetViews>
@@ -7788,10 +10102,10 @@
       <c r="C4"/>
       <c r="D4"/>
       <c r="E4"/>
-      <c r="F4" s="176" t="s">
+      <c r="F4" s="181" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="177"/>
+      <c r="G4" s="182"/>
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -8731,12 +11045,12 @@
       <c r="U21" s="118"/>
     </row>
     <row r="22" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R22" s="178" t="s">
+      <c r="R22" s="183" t="s">
         <v>68</v>
       </c>
-      <c r="S22" s="179"/>
-      <c r="T22" s="179"/>
-      <c r="U22" s="180"/>
+      <c r="S22" s="184"/>
+      <c r="T22" s="184"/>
+      <c r="U22" s="185"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>